<commit_message>
tblAnsprechpartner alle Daten integeriert und die Importdaten vereinheitlicht.
</commit_message>
<xml_diff>
--- a/0-Datengrundlage/2-Ansprechpartner/Ansprechpartner - Name.xlsx
+++ b/0-Datengrundlage/2-Ansprechpartner/Ansprechpartner - Name.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tricuper\Documents\GitHub\TTSF-Hohberg-Sponsoring\0-Datengrundlage\2-Ansprechpartner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0615964C-842C-418F-8014-CF3958BAA224}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{966C1B5F-7970-492A-9C5F-151C5EA06323}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="63">
-  <si>
-    <t>???</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="62">
   <si>
     <t>Roland Straub</t>
   </si>
@@ -220,36 +217,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="h:mm;@"/>
-  </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -260,7 +234,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -268,47 +242,14 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -587,491 +528,356 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C68"/>
+  <dimension ref="A1:A68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="A61" sqref="A61"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.140625" customWidth="1"/>
-    <col min="2" max="3" width="134.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="4"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="4"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="4"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="4"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="4"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="4"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="4"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="4"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="4"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="4"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="4"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="4"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="4"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="4"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="4"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="4"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="1"/>
-      <c r="C20" s="4"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="1"/>
-      <c r="C21" s="4"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="1"/>
-      <c r="C22" s="4"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>19</v>
       </c>
-      <c r="B23" s="1"/>
-      <c r="C23" s="4"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>20</v>
       </c>
-      <c r="B24" s="1"/>
-      <c r="C24" s="4"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>21</v>
       </c>
-      <c r="B25" s="1"/>
-      <c r="C25" s="4"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>22</v>
       </c>
-      <c r="B26" s="3"/>
-      <c r="C26" s="4"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>23</v>
       </c>
-      <c r="B27" s="2"/>
-      <c r="C27" s="4"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>24</v>
       </c>
-      <c r="B28" s="3"/>
-      <c r="C28" s="4"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>25</v>
       </c>
-      <c r="B29" s="3"/>
-      <c r="C29" s="4"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="2"/>
-      <c r="C30" s="4"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>27</v>
       </c>
-      <c r="B31" s="3"/>
-      <c r="C31" s="4"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>28</v>
       </c>
-      <c r="B32" s="1"/>
-      <c r="C32" s="3"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>29</v>
       </c>
-      <c r="B33" s="1"/>
-      <c r="C33" s="4"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>30</v>
       </c>
-      <c r="B34" s="1"/>
-      <c r="C34" s="4"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>31</v>
       </c>
-      <c r="B35" s="1"/>
-      <c r="C35" s="4"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>32</v>
       </c>
-      <c r="B36" s="2"/>
-      <c r="C36" s="4"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>33</v>
       </c>
-      <c r="B37" s="3"/>
-      <c r="C37" s="4"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>34</v>
       </c>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>35</v>
       </c>
-      <c r="B39" s="1"/>
-      <c r="C39" s="4"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>36</v>
       </c>
-      <c r="B40" s="1"/>
-      <c r="C40" s="4"/>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>37</v>
       </c>
-      <c r="B41" s="1"/>
-      <c r="C41" s="4"/>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>38</v>
       </c>
-      <c r="B42" s="1"/>
-      <c r="C42" s="4"/>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>39</v>
       </c>
-      <c r="B43" s="2"/>
-      <c r="C43" s="4"/>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>40</v>
       </c>
-      <c r="B44" s="1"/>
-      <c r="C44" s="4"/>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>41</v>
       </c>
-      <c r="B45" s="1"/>
-      <c r="C45" s="4"/>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>42</v>
       </c>
-      <c r="B46" s="3"/>
-      <c r="C46" s="4"/>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B47" s="1"/>
-      <c r="C47" s="1"/>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>43</v>
       </c>
-      <c r="B48" s="1"/>
-      <c r="C48" s="4"/>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B49" s="1"/>
-      <c r="C49" s="4"/>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>44</v>
       </c>
-      <c r="B50" s="1"/>
-      <c r="C50" s="1"/>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>45</v>
       </c>
-      <c r="B51" s="3"/>
-      <c r="C51" s="4"/>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>46</v>
       </c>
-      <c r="B52" s="1"/>
-      <c r="C52" s="1"/>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>47</v>
       </c>
-      <c r="B53" s="1"/>
-      <c r="C53" s="4"/>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B54" s="1"/>
-      <c r="C54" s="1"/>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>48</v>
       </c>
-      <c r="B55" s="1"/>
-      <c r="C55" s="4"/>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>49</v>
       </c>
-      <c r="B56" s="1"/>
-      <c r="C56" s="4"/>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>50</v>
       </c>
-      <c r="B57" s="3"/>
-      <c r="C57" s="4"/>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
         <v>51</v>
       </c>
-      <c r="B58" s="1"/>
-      <c r="C58" s="4"/>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
         <v>52</v>
       </c>
-      <c r="B59" s="1"/>
-      <c r="C59" s="4"/>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
         <v>53</v>
       </c>
-      <c r="B60" s="1"/>
-      <c r="C60" s="4"/>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B61" s="1"/>
-      <c r="C61" s="1"/>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>54</v>
       </c>
-      <c r="B62" s="3"/>
-      <c r="C62" s="4"/>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>55</v>
       </c>
-      <c r="B63" s="1"/>
-      <c r="C63" s="4"/>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>56</v>
       </c>
-      <c r="B64" s="1"/>
-      <c r="C64" s="4"/>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
         <v>57</v>
       </c>
-      <c r="B65" s="1"/>
-      <c r="C65" s="4"/>
-    </row>
-    <row r="66" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>58</v>
       </c>
-      <c r="B66" s="3"/>
-      <c r="C66" s="4"/>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
         <v>59</v>
       </c>
-      <c r="B67" s="3"/>
-      <c r="C67" s="4"/>
-    </row>
-    <row r="68" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B68" s="3"/>
-      <c r="C68" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>